<commit_message>
fake data for testing purposes
</commit_message>
<xml_diff>
--- a/brands/000001.xlsx
+++ b/brands/000001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsizo\OneDrive\Documents\GitHub\size-adviser-server\brands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3ED00E0A-79A7-475A-8689-0750B236FC1B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCE9407-0F43-4F46-B210-E8855DF77A95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2505" yWindow="1185" windowWidth="15375" windowHeight="7830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Brand</t>
   </si>
@@ -59,7 +59,7 @@
     <t>Adidas</t>
   </si>
   <si>
-    <t>f</t>
+    <t>m</t>
   </si>
 </sst>
 </file>
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,6 +450,47 @@
         <v>38</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>37</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="E4">
+        <v>5.5</v>
+      </c>
+      <c r="F4" t="str">
+        <f>"38 1/3"</f>
+        <v>38 1/3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <v>37.5</v>
+      </c>
+      <c r="D5">
+        <v>7.5</v>
+      </c>
+      <c r="E5">
+        <v>6</v>
+      </c>
+      <c r="F5">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
+1 fake row (test)
</commit_message>
<xml_diff>
--- a/brands/000001.xlsx
+++ b/brands/000001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsizo\OneDrive\Documents\GitHub\size-adviser-server\brands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BCE9407-0F43-4F46-B210-E8855DF77A95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA2ADDF-6229-415B-94F3-DC5AA5F1997C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2505" yWindow="1185" windowWidth="15375" windowHeight="7830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
   <si>
     <t>Brand</t>
   </si>
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,17 +417,16 @@
         <v>8</v>
       </c>
       <c r="C2">
-        <v>36</v>
+        <v>35.5</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>5.5</v>
       </c>
       <c r="E2">
-        <v>4.5</v>
-      </c>
-      <c r="F2" s="1" t="str">
-        <f>"37 1/3"</f>
-        <v>37 1/3</v>
+        <v>4</v>
+      </c>
+      <c r="F2" s="1">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -438,16 +437,17 @@
         <v>8</v>
       </c>
       <c r="C3">
-        <v>36.5</v>
+        <v>36</v>
       </c>
       <c r="D3">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="E3">
-        <v>5</v>
-      </c>
-      <c r="F3">
-        <v>38</v>
+        <v>4.5</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f>"37 1/3"</f>
+        <v>37 1/3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -458,17 +458,16 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>37</v>
+        <v>36.5</v>
       </c>
       <c r="D4">
-        <v>7</v>
+        <v>6.5</v>
       </c>
       <c r="E4">
-        <v>5.5</v>
-      </c>
-      <c r="F4" t="str">
-        <f>"38 1/3"</f>
-        <v>38 1/3</v>
+        <v>5</v>
+      </c>
+      <c r="F4">
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -479,15 +478,36 @@
         <v>8</v>
       </c>
       <c r="C5">
+        <v>37</v>
+      </c>
+      <c r="D5">
+        <v>7</v>
+      </c>
+      <c r="E5">
+        <v>5.5</v>
+      </c>
+      <c r="F5" t="str">
+        <f>"38 1/3"</f>
+        <v>38 1/3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6">
         <v>37.5</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>7.5</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>6</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>39</v>
       </c>
     </row>

</xml_diff>

<commit_message>
more fake records (test)
</commit_message>
<xml_diff>
--- a/brands/000001.xlsx
+++ b/brands/000001.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fsizo\OneDrive\Documents\GitHub\size-adviser-server\brands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FA2ADDF-6229-415B-94F3-DC5AA5F1997C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB3ABB4-E3CB-42F0-9405-2C9B331E86C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2505" yWindow="1185" windowWidth="15375" windowHeight="7830" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="10">
   <si>
     <t>Brand</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>m</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -378,10 +381,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,6 +514,108 @@
         <v>39</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>35.5</v>
+      </c>
+      <c r="D7">
+        <v>5.5</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>36</v>
+      </c>
+      <c r="D8">
+        <v>6</v>
+      </c>
+      <c r="E8">
+        <v>4.5</v>
+      </c>
+      <c r="F8" s="1" t="str">
+        <f>"37 1/3"</f>
+        <v>37 1/3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>36.5</v>
+      </c>
+      <c r="D9">
+        <v>6.5</v>
+      </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
+      <c r="F9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>37</v>
+      </c>
+      <c r="D10">
+        <v>7</v>
+      </c>
+      <c r="E10">
+        <v>5.5</v>
+      </c>
+      <c r="F10" t="str">
+        <f>"38 1/3"</f>
+        <v>38 1/3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>37.5</v>
+      </c>
+      <c r="D11">
+        <v>7.5</v>
+      </c>
+      <c r="E11">
+        <v>6</v>
+      </c>
+      <c r="F11">
+        <v>39</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>